<commit_message>
Lab Exam Backtracking mod
</commit_message>
<xml_diff>
--- a/bin/Marks.xlsx
+++ b/bin/Marks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\alg-2-RicoIglesiasMateo-UO277172\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE756FD-E463-438C-92E5-E2312C205C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA348D12-E240-4082-A543-9CD5FEF753CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Lab 0, 1.1, 1.2</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>Division1		 a=1; b=3; k=1; O(n). Substraction4 waste of stack is O(n)</t>
+  </si>
+  <si>
+    <t>The complexity would be O(countries + borders*colors). You can also consider the number of colors constant if they never change, so the complexity would be just O(countries + borders).</t>
+  </si>
+  <si>
+    <t>Very good. Please, use PDF version of the documents. It would make more sense to indicate the specific examples in the Test class, not in the implementation one.</t>
+  </si>
+  <si>
+    <t>Bactracking has a O(3^n) complexity. You got some weird values sometimes (backrtacking pruning (with balancing condition) cannot be better than backtracking without pruning in any case</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1025,7 @@
   <dimension ref="A1:J138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1080,7 +1089,7 @@
       </c>
       <c r="J4" s="13">
         <f>B6*B4+C6*C4+D6*D4+E6*E4+F6*F4+G6*G4+H6*H4</f>
-        <v>2.9874999999999998</v>
+        <v>7.6374999999999993</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -1128,14 +1137,20 @@
       <c r="D6" s="9">
         <v>9.25</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="E6" s="9">
+        <v>9.5</v>
+      </c>
+      <c r="F6" s="9">
+        <v>9.5</v>
+      </c>
+      <c r="G6" s="9">
+        <v>9</v>
+      </c>
       <c r="H6" s="9"/>
       <c r="I6" s="12"/>
       <c r="J6" s="10">
         <f>IF(J4&lt;5,J4,IF(J4&lt;6,5,IF(J4&lt;7,5.5,IF(J4&lt;8,6,IF(J4&lt;9,6.5,IF(J4&lt;=10,7,100))))))</f>
-        <v>2.9874999999999998</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1148,9 +1163,15 @@
       <c r="D7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="E7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
     </row>

</xml_diff>